<commit_message>
Update environment and mock snakemake
</commit_message>
<xml_diff>
--- a/scenarios/ME IRP 2024/sub_scenarios/plant_availability.xlsx
+++ b/scenarios/ME IRP 2024/sub_scenarios/plant_availability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\172.29.13.112\Github-shared\pypsa-za2\scenarios\ME IRP 2024\sub_scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF375CA6-8ED2-4CC2-A43E-54A20088B0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A30F0BD-6939-4279-B2A7-C9DE94F2BF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="135" yWindow="855" windowWidth="28665" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="annual_availability" sheetId="2" r:id="rId1"/>
@@ -46629,8 +46629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7914E6-3A7F-4107-9EA4-9CE2DF0AD932}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AC12" sqref="AC12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46962,127 +46962,127 @@
         <v>84</v>
       </c>
       <c r="D4" s="20">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E4" s="20">
         <f>D4</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F4" s="20">
         <f>E4</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G4" s="20">
         <f t="shared" ref="G4:AH4" si="0">F4</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="L4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="R4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="T4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="U4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="V4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="W4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="X4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Y4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Z4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AA4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AB4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AC4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AD4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AE4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AF4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AG4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AH4" s="20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>